<commit_message>
Revise and add detail to FSM diagram
</commit_message>
<xml_diff>
--- a/FSM_Diagram/Mouse2AFC_State_Tranition_Table.xlsx
+++ b/FSM_Diagram/Mouse2AFC_State_Tranition_Table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hflyn\Bpod-Coop\FSM_Diagram\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hflyn\Bpod-Coop\mouse2afc\FSM_Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47FDBF8-EE9C-459A-B818-38E69C842E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00811767-7435-4A49-9EC1-C6FA5A688130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="69">
   <si>
     <t>SOURCE</t>
   </si>
@@ -61,18 +61,9 @@
     <t>9. early_withdraw</t>
   </si>
   <si>
-    <t>10.BeepMinSampling</t>
-  </si>
-  <si>
-    <t>25.timeOut_EarlyWithdraw</t>
-  </si>
-  <si>
     <t>26. timeOut_EarlyWithdrawFlashOn</t>
   </si>
   <si>
-    <t>30.ITI</t>
-  </si>
-  <si>
     <t>'SoftCode1'</t>
   </si>
   <si>
@@ -157,9 +148,6 @@
     <t>19. WaitRewardOut</t>
   </si>
   <si>
-    <t>31. ext.ITI</t>
-  </si>
-  <si>
     <t>Exit</t>
   </si>
   <si>
@@ -233,6 +221,12 @@
   </si>
   <si>
     <t>GlobalTimer4_end</t>
+  </si>
+  <si>
+    <t>10. BeepMinSampling</t>
+  </si>
+  <si>
+    <t>25. timeOut_EarlyWithdraw</t>
   </si>
 </sst>
 </file>
@@ -2821,7 +2815,7 @@
   <dimension ref="A1:C62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2849,7 +2843,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -2871,7 +2865,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -2882,7 +2876,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -2901,7 +2895,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -2917,10 +2911,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -2928,48 +2922,48 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -2985,37 +2979,37 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
         <v>10</v>
@@ -3023,29 +3017,29 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C22" t="s">
         <v>10</v>
@@ -3053,10 +3047,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C23" t="s">
         <v>10</v>
@@ -3064,164 +3058,164 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" t="s">
         <v>20</v>
       </c>
-      <c r="B28" t="s">
-        <v>23</v>
-      </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C30" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C31" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B34" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C34" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B35" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C35" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B36" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C36" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C37" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" t="s">
         <v>33</v>
-      </c>
-      <c r="B38" t="s">
-        <v>32</v>
-      </c>
-      <c r="C38" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C39" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C40" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
@@ -3229,121 +3223,121 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C42" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>32</v>
+      </c>
+      <c r="B43" t="s">
         <v>35</v>
       </c>
-      <c r="B43" t="s">
-        <v>38</v>
-      </c>
       <c r="C43" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" t="s">
         <v>59</v>
-      </c>
-      <c r="C44" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C45" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B46" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C46" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C47" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B48" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C48" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B49" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C49" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C50" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B51" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C51" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C52" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C53" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C54" t="s">
         <v>6</v>
@@ -3351,81 +3345,81 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C55" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B56" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C56" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B57" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C57" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B58" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C58" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C59" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B60" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C60" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B61" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C61" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C62" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>